<commit_message>
add exam to database and retrieve exam
</commit_message>
<xml_diff>
--- a/files/exams.xlsx
+++ b/files/exams.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\online exam and grading system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\online exam and grading system\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>total_marks</t>
   </si>
@@ -44,19 +44,34 @@
     <t>end_time</t>
   </si>
   <si>
-    <t>Physics Practical</t>
-  </si>
-  <si>
-    <t>English Midterm</t>
-  </si>
-  <si>
-    <t>Biology Final</t>
-  </si>
-  <si>
     <t>UT01</t>
   </si>
   <si>
-    <t>UT01_social</t>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>ut02</t>
+  </si>
+  <si>
+    <t>ut01</t>
+  </si>
+  <si>
+    <t>ut03</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>physics</t>
+  </si>
+  <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t>chemisrty</t>
+  </si>
+  <si>
+    <t>ip</t>
   </si>
 </sst>
 </file>
@@ -380,19 +395,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -400,115 +417,133 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>501</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
         <v>101</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>100</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>0.375</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>502</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1">
         <v>102</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>150</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>503</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1">
         <v>103</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>50</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>504</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1">
         <v>104</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>80</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>505</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1">
         <v>105</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>120</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>0.66666666666666663</v>
       </c>
     </row>

</xml_diff>